<commit_message>
identify clubs from 2004
identify clubs from 2004
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="332">
   <si>
     <t>Logt for total gdppc</t>
   </si>
@@ -168,6 +168,21 @@
     <t>Club14</t>
   </si>
   <si>
+    <t>Club15</t>
+  </si>
+  <si>
+    <t>Club16</t>
+  </si>
+  <si>
+    <t>Club17</t>
+  </si>
+  <si>
+    <t>Club18</t>
+  </si>
+  <si>
+    <t>Group19</t>
+  </si>
+  <si>
     <t>Initial Clubs for agriculture gdp</t>
   </si>
   <si>
@@ -378,7 +393,28 @@
     <t>Club67</t>
   </si>
   <si>
-    <t>Group68</t>
+    <t>Club68</t>
+  </si>
+  <si>
+    <t>Club69</t>
+  </si>
+  <si>
+    <t>Club70</t>
+  </si>
+  <si>
+    <t>Club71</t>
+  </si>
+  <si>
+    <t>Club72</t>
+  </si>
+  <si>
+    <t>Club73</t>
+  </si>
+  <si>
+    <t>Club74</t>
+  </si>
+  <si>
+    <t>Group75</t>
   </si>
   <si>
     <t>Merging Clubs for total gdppc</t>
@@ -480,6 +516,18 @@
     <t>Club13+14</t>
   </si>
   <si>
+    <t>Club14+15</t>
+  </si>
+  <si>
+    <t>Club15+16</t>
+  </si>
+  <si>
+    <t>Club16+17</t>
+  </si>
+  <si>
+    <t>Club17+18</t>
+  </si>
+  <si>
     <t>Merging Clubs for agriculture gdp</t>
   </si>
   <si>
@@ -687,6 +735,27 @@
     <t>Club66+67</t>
   </si>
   <si>
+    <t>Club67+68</t>
+  </si>
+  <si>
+    <t>Club68+69</t>
+  </si>
+  <si>
+    <t>Club69+70</t>
+  </si>
+  <si>
+    <t>Club70+71</t>
+  </si>
+  <si>
+    <t>Club71+72</t>
+  </si>
+  <si>
+    <t>Club72+73</t>
+  </si>
+  <si>
+    <t>Club73+74</t>
+  </si>
+  <si>
     <t>Final Clubs for total gdppc</t>
   </si>
   <si>
@@ -741,6 +810,18 @@
     <t>Club6</t>
   </si>
   <si>
+    <t>Club7</t>
+  </si>
+  <si>
+    <t>Club8</t>
+  </si>
+  <si>
+    <t>Club9</t>
+  </si>
+  <si>
+    <t>Group10</t>
+  </si>
+  <si>
     <t>Final Clubs for agriculture gdp</t>
   </si>
   <si>
@@ -885,7 +966,52 @@
     <t>Club45</t>
   </si>
   <si>
-    <t>Group46</t>
+    <t>Club46</t>
+  </si>
+  <si>
+    <t>Club47</t>
+  </si>
+  <si>
+    <t>Club48</t>
+  </si>
+  <si>
+    <t>Club49</t>
+  </si>
+  <si>
+    <t>Club50</t>
+  </si>
+  <si>
+    <t>Club51</t>
+  </si>
+  <si>
+    <t>Club52</t>
+  </si>
+  <si>
+    <t>Club53</t>
+  </si>
+  <si>
+    <t>Club54</t>
+  </si>
+  <si>
+    <t>Club55</t>
+  </si>
+  <si>
+    <t>Club56</t>
+  </si>
+  <si>
+    <t>Club57</t>
+  </si>
+  <si>
+    <t>Club58</t>
+  </si>
+  <si>
+    <t>Club59</t>
+  </si>
+  <si>
+    <t>Club60</t>
+  </si>
+  <si>
+    <t>Group61</t>
   </si>
 </sst>
 </file>
@@ -1629,13 +1755,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="4">
-        <v>-0.54923773737202519</v>
+        <v>-0.65779183644215855</v>
       </c>
       <c r="C3" s="4">
-        <v>0.022950158755856452</v>
+        <v>0.024871171147408989</v>
       </c>
       <c r="D3" s="4">
-        <v>-23.931762007174349</v>
+        <v>-26.447963891345967</v>
       </c>
     </row>
     <row r="6">
@@ -1660,13 +1786,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="8">
-        <v>-0.47380562746515054</v>
+        <v>-0.61358256357937091</v>
       </c>
       <c r="C8" s="8">
-        <v>0.020675814019332332</v>
+        <v>0.025675528705082808</v>
       </c>
       <c r="D8" s="8">
-        <v>-22.91593583798597</v>
+        <v>-23.897562952925842</v>
       </c>
     </row>
     <row r="11">
@@ -1691,13 +1817,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="12">
-        <v>-0.5097713550073788</v>
+        <v>-0.63333811419791508</v>
       </c>
       <c r="C13" s="12">
-        <v>0.022625466078812453</v>
+        <v>0.026790540812152853</v>
       </c>
       <c r="D13" s="12">
-        <v>-22.530866468415102</v>
+        <v>-23.640363165442977</v>
       </c>
     </row>
   </sheetData>
@@ -1706,7 +1832,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BQ15"/>
+  <dimension ref="A1:BX15"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -1767,49 +1893,49 @@
         <v>16</v>
       </c>
       <c r="B3" s="16">
-        <v>0.16056846624037902</v>
+        <v>0.070880798450786764</v>
       </c>
       <c r="C3" s="16">
-        <v>0.2020266654693974</v>
+        <v>-0.0014577708825504465</v>
       </c>
       <c r="D3" s="16">
-        <v>0.10601712678479358</v>
+        <v>0.038740664598068075</v>
       </c>
       <c r="E3" s="16">
-        <v>0.030415375699979263</v>
+        <v>0.076400142346895072</v>
       </c>
       <c r="F3" s="16">
-        <v>0.06577094750613699</v>
+        <v>0.11544528956556446</v>
       </c>
       <c r="G3" s="16">
-        <v>0.0067625147689597265</v>
+        <v>0.069283968840283594</v>
       </c>
       <c r="H3" s="16">
-        <v>0.02573710445963906</v>
+        <v>0.057400311110860636</v>
       </c>
       <c r="I3" s="16">
-        <v>0.053921575613319839</v>
+        <v>0.045002598000372984</v>
       </c>
       <c r="J3" s="16">
-        <v>0.088695462489084331</v>
+        <v>0.058619582057811426</v>
       </c>
       <c r="K3" s="16">
-        <v>0.060246213747008448</v>
+        <v>0.12611581065112137</v>
       </c>
       <c r="L3" s="16">
-        <v>0.057514047187250783</v>
+        <v>0.16435184736648181</v>
       </c>
       <c r="M3" s="16">
-        <v>0.081702421163455274</v>
+        <v>0.20180756515868031</v>
       </c>
       <c r="N3" s="16">
-        <v>0.099588101869396761</v>
+        <v>0.24592857984645031</v>
       </c>
       <c r="O3" s="16">
-        <v>0.04317559990045261</v>
+        <v>0.08678961267934085</v>
       </c>
       <c r="P3" s="16">
-        <v>0.076406335660846925</v>
+        <v>0.094271373264193881</v>
       </c>
     </row>
     <row r="4">
@@ -1817,49 +1943,49 @@
         <v>17</v>
       </c>
       <c r="B4" s="16">
-        <v>2.0892865872558959</v>
+        <v>0.94249337269788314</v>
       </c>
       <c r="C4" s="16">
-        <v>2.6933046938668381</v>
+        <v>-0.027670210256611438</v>
       </c>
       <c r="D4" s="16">
-        <v>1.5019339019387599</v>
+        <v>0.48035163516136842</v>
       </c>
       <c r="E4" s="16">
-        <v>0.45705092240310141</v>
+        <v>1.0202631747441759</v>
       </c>
       <c r="F4" s="16">
-        <v>0.96817738164346356</v>
+        <v>1.5076842345140642</v>
       </c>
       <c r="G4" s="16">
-        <v>0.10306020913963009</v>
+        <v>0.86612491116259593</v>
       </c>
       <c r="H4" s="16">
-        <v>0.4013031432127418</v>
+        <v>0.71391044893891464</v>
       </c>
       <c r="I4" s="16">
-        <v>0.8520930351480952</v>
+        <v>0.58918732257403306</v>
       </c>
       <c r="J4" s="16">
-        <v>1.2843935387723364</v>
+        <v>0.7426331151983534</v>
       </c>
       <c r="K4" s="16">
-        <v>0.92694558817961392</v>
+        <v>1.6116894137836477</v>
       </c>
       <c r="L4" s="16">
-        <v>0.89711972079912805</v>
+        <v>1.983567768844493</v>
       </c>
       <c r="M4" s="16">
-        <v>1.3634572874538604</v>
+        <v>2.500802113691643</v>
       </c>
       <c r="N4" s="16">
-        <v>1.487708281086308</v>
+        <v>2.923503719951035</v>
       </c>
       <c r="O4" s="16">
-        <v>0.74194285038838914</v>
+        <v>1.2488423294053337</v>
       </c>
       <c r="P4" s="16">
-        <v>1.3540300232200393</v>
+        <v>1.5932464753855013</v>
       </c>
     </row>
     <row r="6">
@@ -1911,52 +2037,82 @@
       <c r="O7" s="20" t="s">
         <v>49</v>
       </c>
+      <c r="P7" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q7" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="R7" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="S7" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="T7" s="20" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="20" t="s">
         <v>34</v>
       </c>
       <c r="B8" s="20">
-        <v>0.41573624195788395</v>
+        <v>0.4460402346943792</v>
       </c>
       <c r="C8" s="20">
-        <v>0.16352016084591958</v>
+        <v>0.13747629301234462</v>
       </c>
       <c r="D8" s="20">
-        <v>0.06590183502405017</v>
+        <v>0.17019563014822001</v>
       </c>
       <c r="E8" s="20">
-        <v>0.11257828390700569</v>
+        <v>0.026391178041429042</v>
       </c>
       <c r="F8" s="20">
-        <v>0.10920342337652028</v>
+        <v>0.053064121914309259</v>
       </c>
       <c r="G8" s="20">
-        <v>0.12632322101467477</v>
+        <v>0.066071298569613413</v>
       </c>
       <c r="H8" s="20">
-        <v>0.081098883821636658</v>
+        <v>0.080005099897608067</v>
       </c>
       <c r="I8" s="20">
-        <v>0.24484432266804881</v>
+        <v>0.038204052219218354</v>
       </c>
       <c r="J8" s="20">
-        <v>0.036314916859046587</v>
+        <v>0.085842304672390707</v>
       </c>
       <c r="K8" s="20">
-        <v>0.074186008685923344</v>
+        <v>0.10832520029947212</v>
       </c>
       <c r="L8" s="20">
-        <v>0.13194741414607444</v>
+        <v>0.088667031546551867</v>
       </c>
       <c r="M8" s="20">
-        <v>0.054704714263936527</v>
+        <v>0.10143298317319926</v>
       </c>
       <c r="N8" s="20">
-        <v>0.19751623790844089</v>
+        <v>0.20529462380183833</v>
       </c>
       <c r="O8" s="20">
-        <v>0.05550848555641244</v>
+        <v>0.077757621865667315</v>
+      </c>
+      <c r="P8" s="20">
+        <v>0.12589352760709618</v>
+      </c>
+      <c r="Q8" s="20">
+        <v>0.09342844444573814</v>
+      </c>
+      <c r="R8" s="20">
+        <v>0.25520356178774189</v>
+      </c>
+      <c r="S8" s="20">
+        <v>0.026094157395636752</v>
+      </c>
+      <c r="T8" s="20">
+        <v>-0.70277563076210114</v>
       </c>
     </row>
     <row r="9">
@@ -1964,676 +2120,754 @@
         <v>35</v>
       </c>
       <c r="B9" s="20">
-        <v>5.323540716719088</v>
+        <v>4.5526621331696351</v>
       </c>
       <c r="C9" s="20">
-        <v>2.5513765553897296</v>
+        <v>2.4891705499557344</v>
       </c>
       <c r="D9" s="20">
-        <v>1.1468028263710937</v>
+        <v>2.3949246130938042</v>
       </c>
       <c r="E9" s="20">
-        <v>1.7800963856660006</v>
+        <v>0.39267496441654287</v>
       </c>
       <c r="F9" s="20">
-        <v>1.8871223418717809</v>
+        <v>0.74618878328689875</v>
       </c>
       <c r="G9" s="20">
-        <v>2.1658374846983288</v>
+        <v>0.94350557468195873</v>
       </c>
       <c r="H9" s="20">
-        <v>1.5705505520796934</v>
+        <v>1.1157900929695015</v>
       </c>
       <c r="I9" s="20">
-        <v>4.1479255392455796</v>
+        <v>0.57980190773897222</v>
       </c>
       <c r="J9" s="20">
-        <v>0.79167065065688802</v>
+        <v>1.2297128506951747</v>
       </c>
       <c r="K9" s="20">
-        <v>1.2687013442340946</v>
+        <v>1.5581145236270579</v>
       </c>
       <c r="L9" s="20">
-        <v>2.5564227200823328</v>
+        <v>1.2427729710418436</v>
       </c>
       <c r="M9" s="20">
-        <v>1.1434375040999336</v>
+        <v>1.4095061850719668</v>
       </c>
       <c r="N9" s="20">
-        <v>4.1340411038147868</v>
+        <v>2.8831677280035573</v>
       </c>
       <c r="O9" s="20">
-        <v>1.737333029694796</v>
+        <v>1.1263739315932058</v>
+      </c>
+      <c r="P9" s="20">
+        <v>1.9326677758379809</v>
+      </c>
+      <c r="Q9" s="20">
+        <v>1.4912821377912004</v>
+      </c>
+      <c r="R9" s="20">
+        <v>3.53915153848145</v>
+      </c>
+      <c r="S9" s="20">
+        <v>0.47126308037296438</v>
+      </c>
+      <c r="T9" s="20">
+        <v>-26.413103445171018</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="23" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="24"/>
       <c r="B13" s="24" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="E13" s="24" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="G13" s="24" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="J13" s="24" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="K13" s="24" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="L13" s="24" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="M13" s="24" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="N13" s="24" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="O13" s="24" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="P13" s="24" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="Q13" s="24" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="R13" s="24" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="S13" s="24" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="T13" s="24" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="U13" s="24" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="V13" s="24" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="W13" s="24" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="X13" s="24" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="Y13" s="24" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="Z13" s="24" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="AA13" s="24" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="AB13" s="24" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="AC13" s="24" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="AD13" s="24" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="AE13" s="24" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="AF13" s="24" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="AG13" s="24" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="AH13" s="24" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="AI13" s="24" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="AJ13" s="24" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="AK13" s="24" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="AL13" s="24" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="AM13" s="24" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="AN13" s="24" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="AO13" s="24" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="AP13" s="24" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="AQ13" s="24" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="AR13" s="24" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="AS13" s="24" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="AT13" s="24" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="AU13" s="24" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="AV13" s="24" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="AW13" s="24" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="AX13" s="24" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="AY13" s="24" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="AZ13" s="24" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="BA13" s="24" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="BB13" s="24" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="BC13" s="24" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="BD13" s="24" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="BE13" s="24" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="BF13" s="24" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="BG13" s="24" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="BH13" s="24" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="BI13" s="24" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="BJ13" s="24" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="BK13" s="24" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="BL13" s="24" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="BM13" s="24" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="BN13" s="24" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="BO13" s="24" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="BP13" s="24" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="BQ13" s="24" t="s">
-        <v>120</v>
+        <v>125</v>
+      </c>
+      <c r="BR13" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="BS13" s="24" t="s">
+        <v>127</v>
+      </c>
+      <c r="BT13" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="BU13" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="BV13" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="BW13" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="BX13" s="24" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="24" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B14" s="24">
-        <v>0.66962679906595168</v>
+        <v>0.49518170056294702</v>
       </c>
       <c r="C14" s="24">
-        <v>0.13362446219824239</v>
+        <v>0.43660330496016997</v>
       </c>
       <c r="D14" s="24">
-        <v>-2.2166799685721577</v>
+        <v>0.40247902674893671</v>
       </c>
       <c r="E14" s="24">
-        <v>0.0033577666985339372</v>
+        <v>0.33778266276375463</v>
       </c>
       <c r="F14" s="24">
-        <v>0.46095915825999284</v>
+        <v>0.66655483734855214</v>
       </c>
       <c r="G14" s="24">
-        <v>0.12794518942645258</v>
+        <v>0.40244288183093951</v>
       </c>
       <c r="H14" s="24">
-        <v>0.058516117875385021</v>
+        <v>0.061000701347620312</v>
       </c>
       <c r="I14" s="24">
-        <v>-0.012899140648568369</v>
+        <v>0.37482521237543265</v>
       </c>
       <c r="J14" s="24">
-        <v>0.25449849154051812</v>
+        <v>-0.063537241189347615</v>
       </c>
       <c r="K14" s="24">
-        <v>0.15789019950121011</v>
+        <v>1.2952089302737855</v>
       </c>
       <c r="L14" s="24">
-        <v>0.18450513416916531</v>
+        <v>0.062049656090342603</v>
       </c>
       <c r="M14" s="24">
-        <v>0.029350881801036122</v>
+        <v>0.14897427922432865</v>
       </c>
       <c r="N14" s="24">
-        <v>0.36696500674523652</v>
+        <v>0.61840952009149741</v>
       </c>
       <c r="O14" s="24">
-        <v>-0.014189755919901792</v>
+        <v>0.087195437588785285</v>
       </c>
       <c r="P14" s="24">
-        <v>-0.095461834978672278</v>
+        <v>1.5874525706655915</v>
       </c>
       <c r="Q14" s="24">
-        <v>0.072397055807492949</v>
+        <v>0.29921784466845747</v>
       </c>
       <c r="R14" s="24">
-        <v>0.30230795563842894</v>
+        <v>0.055490230771631399</v>
       </c>
       <c r="S14" s="24">
-        <v>0.079262888795319453</v>
+        <v>-0.12390894052888557</v>
       </c>
       <c r="T14" s="24">
-        <v>0.24584638669417613</v>
+        <v>-0.13578999200336792</v>
       </c>
       <c r="U14" s="24">
-        <v>0.30442226496706593</v>
+        <v>0.018916687568856227</v>
       </c>
       <c r="V14" s="24">
-        <v>0.2882601262266633</v>
+        <v>-0.024419501588821835</v>
       </c>
       <c r="W14" s="24">
-        <v>0.14712879788177241</v>
+        <v>0.063386533603545903</v>
       </c>
       <c r="X14" s="24">
-        <v>0.098925034977034643</v>
+        <v>0.41105129988779354</v>
       </c>
       <c r="Y14" s="24">
-        <v>0.043434867962179269</v>
+        <v>0.11962688664925708</v>
       </c>
       <c r="Z14" s="24">
-        <v>0.052429032503363504</v>
+        <v>0.23307218060099349</v>
       </c>
       <c r="AA14" s="24">
-        <v>0.42156882376652183</v>
+        <v>0.10889007735635536</v>
       </c>
       <c r="AB14" s="24">
-        <v>0.0046649449889635264</v>
+        <v>0.25827484068170958</v>
       </c>
       <c r="AC14" s="24">
-        <v>0.24320236202728088</v>
+        <v>0.26815435748222377</v>
       </c>
       <c r="AD14" s="24">
-        <v>0.28886838338257576</v>
+        <v>0.046261858286910984</v>
       </c>
       <c r="AE14" s="24">
-        <v>0.17741162426036461</v>
+        <v>0.15560081127923739</v>
       </c>
       <c r="AF14" s="24">
-        <v>0.89420088651386331</v>
+        <v>0.043717421558212399</v>
       </c>
       <c r="AG14" s="24">
-        <v>0.044156608111483586</v>
+        <v>0.23892754274016009</v>
       </c>
       <c r="AH14" s="24">
-        <v>0.10062229888943536</v>
+        <v>0.16939603298637362</v>
       </c>
       <c r="AI14" s="24">
-        <v>0.073916254253936858</v>
+        <v>0.014132020740962536</v>
       </c>
       <c r="AJ14" s="24">
-        <v>0.13002709607720137</v>
+        <v>0.13088052993207011</v>
       </c>
       <c r="AK14" s="24">
-        <v>0.36171660393626837</v>
+        <v>0.13573161174637211</v>
       </c>
       <c r="AL14" s="24">
-        <v>0.041746887107786512</v>
+        <v>0.053775657491802686</v>
       </c>
       <c r="AM14" s="24">
-        <v>0.1688042656237598</v>
+        <v>1.2220119486591683</v>
       </c>
       <c r="AN14" s="24">
-        <v>0.19986301583214405</v>
+        <v>0.019477750354321088</v>
       </c>
       <c r="AO14" s="24">
-        <v>0.2373428459627068</v>
+        <v>0.37426538949707044</v>
       </c>
       <c r="AP14" s="24">
-        <v>0.046698070105317346</v>
+        <v>-0.036145729835015017</v>
       </c>
       <c r="AQ14" s="24">
-        <v>0.04933201594730624</v>
+        <v>0.18368003790265566</v>
       </c>
       <c r="AR14" s="24">
-        <v>0.1079668930763977</v>
+        <v>0.08205232765447884</v>
       </c>
       <c r="AS14" s="24">
-        <v>0.087932836373407319</v>
+        <v>0.32349990356091229</v>
       </c>
       <c r="AT14" s="24">
-        <v>0.62959165601735156</v>
+        <v>0.080632706242253882</v>
       </c>
       <c r="AU14" s="24">
-        <v>0.091506883198144817</v>
+        <v>0.12235502989365993</v>
       </c>
       <c r="AV14" s="24">
-        <v>0.11526078322588507</v>
+        <v>1.9061611065636717</v>
       </c>
       <c r="AW14" s="24">
-        <v>0.27472198123847019</v>
+        <v>-0.022726000888747822</v>
       </c>
       <c r="AX14" s="24">
-        <v>0.51022042714299998</v>
+        <v>-0.038920704285130947</v>
       </c>
       <c r="AY14" s="24">
-        <v>0.16199262893304092</v>
+        <v>0.10255500476472745</v>
       </c>
       <c r="AZ14" s="24">
-        <v>0.032070244359580224</v>
+        <v>0.092348078919478299</v>
       </c>
       <c r="BA14" s="24">
-        <v>0.13776093774112988</v>
+        <v>0.26929472764911699</v>
       </c>
       <c r="BB14" s="24">
-        <v>0.098251919238211416</v>
+        <v>0.13585726223229622</v>
       </c>
       <c r="BC14" s="24">
-        <v>0.081067212115278675</v>
+        <v>0.093743874056586129</v>
       </c>
       <c r="BD14" s="24">
-        <v>0.0044277104392809741</v>
+        <v>4.2536005140793574</v>
       </c>
       <c r="BE14" s="24">
-        <v>-0.011542843689957172</v>
+        <v>0.13521820435634979</v>
       </c>
       <c r="BF14" s="24">
-        <v>0.64993866141563739</v>
+        <v>0.04347253992499453</v>
       </c>
       <c r="BG14" s="24">
-        <v>0.14339970021016785</v>
+        <v>0.15853831327706275</v>
       </c>
       <c r="BH14" s="24">
-        <v>-0.059624582928452186</v>
+        <v>0.0030973285978477261</v>
       </c>
       <c r="BI14" s="24">
-        <v>0.043933604013526528</v>
+        <v>0.061620758555066296</v>
       </c>
       <c r="BJ14" s="24">
-        <v>3.9904766919570602</v>
+        <v>0.12832135477778733</v>
       </c>
       <c r="BK14" s="24">
-        <v>-0.018699527545565892</v>
+        <v>0.11946085097370376</v>
       </c>
       <c r="BL14" s="24">
-        <v>0.034408885251043825</v>
+        <v>0.72129957436028647</v>
       </c>
       <c r="BM14" s="24">
-        <v>0.53146107928339625</v>
+        <v>1.2370438771579466</v>
       </c>
       <c r="BN14" s="24">
-        <v>0.1228193286704034</v>
+        <v>0.046314345029220605</v>
       </c>
       <c r="BO14" s="24">
-        <v>0.076704474760980385</v>
+        <v>0.094534890745803429</v>
       </c>
       <c r="BP14" s="24">
-        <v>0.10642541921984282</v>
+        <v>0.09869576370038069</v>
       </c>
       <c r="BQ14" s="24">
-        <v>-0.51453561825376026</v>
+        <v>-0.090913474955031659</v>
+      </c>
+      <c r="BR14" s="24">
+        <v>0.073170095455457662</v>
+      </c>
+      <c r="BS14" s="24">
+        <v>0.15833744247497936</v>
+      </c>
+      <c r="BT14" s="24">
+        <v>3.2130627080259062</v>
+      </c>
+      <c r="BU14" s="24">
+        <v>0.47831703403700088</v>
+      </c>
+      <c r="BV14" s="24">
+        <v>0.11958738203699448</v>
+      </c>
+      <c r="BW14" s="24">
+        <v>0.016090794687141585</v>
+      </c>
+      <c r="BX14" s="24">
+        <v>-0.61371963667920859</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="24" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B15" s="24">
-        <v>6.2903470233308614</v>
+        <v>5.2757919361774306</v>
       </c>
       <c r="C15" s="24">
-        <v>2.3653407081514324</v>
+        <v>5.12270890202758</v>
       </c>
       <c r="D15" s="24">
-        <v>-1.6045052331929064</v>
+        <v>5.5110546755875731</v>
       </c>
       <c r="E15" s="24">
-        <v>0.044467710136045405</v>
+        <v>2.7578442892503099</v>
       </c>
       <c r="F15" s="24">
-        <v>5.4430853880501422</v>
+        <v>3.8333227619670605</v>
       </c>
       <c r="G15" s="24">
-        <v>1.9257062541353231</v>
+        <v>7.7384165682239097</v>
       </c>
       <c r="H15" s="24">
-        <v>1.5148819648178191</v>
+        <v>0.64951831536089366</v>
       </c>
       <c r="I15" s="24">
-        <v>-0.7440442222618262</v>
+        <v>4.8900375606575119</v>
       </c>
       <c r="J15" s="24">
-        <v>3.1600949613485949</v>
+        <v>-0.72080875117219512</v>
       </c>
       <c r="K15" s="24">
-        <v>2.2770696037747604</v>
+        <v>9.0739161496455782</v>
       </c>
       <c r="L15" s="24">
-        <v>2.5283248301545505</v>
+        <v>0.87859060827553481</v>
       </c>
       <c r="M15" s="24">
-        <v>0.76903094036502806</v>
+        <v>2.0008293447432481</v>
       </c>
       <c r="N15" s="24">
-        <v>6.1189460068577137</v>
+        <v>0.54849132920819066</v>
       </c>
       <c r="O15" s="24">
-        <v>-0.77745409527881604</v>
+        <v>1.1886690237918631</v>
       </c>
       <c r="P15" s="24">
-        <v>-2.546825420085689</v>
+        <v>20.804839807581164</v>
       </c>
       <c r="Q15" s="24">
-        <v>2.1685100591948494</v>
+        <v>3.3720019659199938</v>
       </c>
       <c r="R15" s="24">
-        <v>4.0269796230726351</v>
+        <v>0.87254745075401619</v>
       </c>
       <c r="S15" s="24">
-        <v>1.8183088726120442</v>
+        <v>-1.9455360921607725</v>
       </c>
       <c r="T15" s="24">
-        <v>3.0585956890836301</v>
+        <v>-0.32191194092089898</v>
       </c>
       <c r="U15" s="24">
-        <v>15.522374012007159</v>
+        <v>0.25586551324184376</v>
       </c>
       <c r="V15" s="24">
-        <v>2.106278418421208</v>
+        <v>-0.4805192613622315</v>
       </c>
       <c r="W15" s="24">
-        <v>2.4115246718502954</v>
+        <v>0.81491090864584914</v>
       </c>
       <c r="X15" s="24">
-        <v>2.1041053663312752</v>
+        <v>3.8174753986433485</v>
       </c>
       <c r="Y15" s="24">
-        <v>0.73985145504026484</v>
+        <v>3.6108759868243294</v>
       </c>
       <c r="Z15" s="24">
-        <v>1.0515380284495321</v>
+        <v>2.3714615937811674</v>
       </c>
       <c r="AA15" s="24">
-        <v>3.262257551243732</v>
+        <v>1.5535018350320537</v>
       </c>
       <c r="AB15" s="24">
-        <v>0.059091751580614568</v>
+        <v>3.7878097717008394</v>
       </c>
       <c r="AC15" s="24">
-        <v>3.6065443594790132</v>
+        <v>1.9327126693475385</v>
       </c>
       <c r="AD15" s="24">
-        <v>3.867872578024417</v>
+        <v>0.65275454049714488</v>
       </c>
       <c r="AE15" s="24">
-        <v>14.272945498637819</v>
+        <v>1.7857474776715805</v>
       </c>
       <c r="AF15" s="24">
-        <v>4.886484973750199</v>
+        <v>0.56237899365208766</v>
       </c>
       <c r="AG15" s="24">
-        <v>1.2070786319943205</v>
+        <v>4.1779918282270696</v>
       </c>
       <c r="AH15" s="24">
-        <v>1.6994446091458872</v>
+        <v>1.2601277230751315</v>
       </c>
       <c r="AI15" s="24">
-        <v>1.904908737219539</v>
+        <v>0.21197253869837085</v>
       </c>
       <c r="AJ15" s="24">
-        <v>0.67769207310114876</v>
+        <v>1.5188647698738706</v>
       </c>
       <c r="AK15" s="24">
-        <v>9.2500018648698745</v>
+        <v>1.4028601972196582</v>
       </c>
       <c r="AL15" s="24">
-        <v>0.77702007302876941</v>
+        <v>0.87684296279163976</v>
       </c>
       <c r="AM15" s="24">
-        <v>3.5204173517908477</v>
+        <v>4.839324812772726</v>
       </c>
       <c r="AN15" s="24">
-        <v>4.4789540484080002</v>
+        <v>0.30219148960457276</v>
       </c>
       <c r="AO15" s="24">
-        <v>5.4951224294678127</v>
+        <v>3.8158409012659584</v>
       </c>
       <c r="AP15" s="24">
-        <v>0.91550820066275795</v>
+        <v>-0.40702402016293432</v>
       </c>
       <c r="AQ15" s="24">
-        <v>1.020890736713439</v>
+        <v>9.0227034262663501</v>
       </c>
       <c r="AR15" s="24">
-        <v>2.2761724082232497</v>
+        <v>4.2406728307232635</v>
       </c>
       <c r="AS15" s="24">
-        <v>2.8629414252873984</v>
+        <v>3.2998528333286852</v>
       </c>
       <c r="AT15" s="24">
-        <v>11.371774700335159</v>
+        <v>1.3056063472488353</v>
       </c>
       <c r="AU15" s="24">
-        <v>1.4496908423054604</v>
+        <v>1.6932185300833573</v>
       </c>
       <c r="AV15" s="24">
-        <v>2.361876666345057</v>
+        <v>9.3743515617708439</v>
       </c>
       <c r="AW15" s="24">
-        <v>3.9945317836019689</v>
+        <v>-0.11052721339930192</v>
       </c>
       <c r="AX15" s="24">
-        <v>7.4354299324933688</v>
+        <v>-0.73400822391863618</v>
       </c>
       <c r="AY15" s="24">
-        <v>3.2244210831444353</v>
+        <v>1.2928952079222877</v>
       </c>
       <c r="AZ15" s="24">
-        <v>0.88013991899990895</v>
+        <v>1.4831038104250389</v>
       </c>
       <c r="BA15" s="24">
-        <v>3.0139705171507831</v>
+        <v>4.2052775292397113</v>
       </c>
       <c r="BB15" s="24">
-        <v>2.006572670984446</v>
+        <v>2.1928990722184047</v>
       </c>
       <c r="BC15" s="24">
-        <v>1.501375431897924</v>
+        <v>1.5936698748363416</v>
       </c>
       <c r="BD15" s="24">
-        <v>0.10782271939116293</v>
+        <v>3.2287534897771093</v>
       </c>
       <c r="BE15" s="24">
-        <v>-0.33938541480762274</v>
+        <v>1.6970337413447576</v>
       </c>
       <c r="BF15" s="24">
-        <v>26.739782456850698</v>
+        <v>1.2045477199314645</v>
       </c>
       <c r="BG15" s="24">
-        <v>7.0314444000588567</v>
+        <v>2.4379253802873579</v>
       </c>
       <c r="BH15" s="24">
-        <v>-1.5715631747374008</v>
+        <v>0.041687198411506872</v>
       </c>
       <c r="BI15" s="24">
-        <v>1.0539250714192765</v>
+        <v>1.5903176832129493</v>
       </c>
       <c r="BJ15" s="24">
-        <v>2.8635183335557635</v>
+        <v>3.0678684791282471</v>
       </c>
       <c r="BK15" s="24">
-        <v>-1.0751371546216089</v>
+        <v>1.9828580554372954</v>
       </c>
       <c r="BL15" s="24">
-        <v>0.85026228636205692</v>
+        <v>7.6732092679835713</v>
       </c>
       <c r="BM15" s="24">
-        <v>6.2881710940480522</v>
+        <v>16.463995213534297</v>
       </c>
       <c r="BN15" s="24">
-        <v>3.4731630142663676</v>
+        <v>0.89229055571995908</v>
       </c>
       <c r="BO15" s="24">
-        <v>3.5923863954045934</v>
+        <v>1.4918734785894916</v>
       </c>
       <c r="BP15" s="24">
-        <v>4.6936959035634578</v>
+        <v>1.5730436655018905</v>
       </c>
       <c r="BQ15" s="24">
-        <v>-22.892776701289684</v>
+        <v>-1.8111827858865415</v>
+      </c>
+      <c r="BR15" s="24">
+        <v>1.7053284187021134</v>
+      </c>
+      <c r="BS15" s="24">
+        <v>2.5575079326147434</v>
+      </c>
+      <c r="BT15" s="24">
+        <v>2.016310711734187</v>
+      </c>
+      <c r="BU15" s="24">
+        <v>5.8815882521741951</v>
+      </c>
+      <c r="BV15" s="24">
+        <v>2.1960558592255399</v>
+      </c>
+      <c r="BW15" s="24">
+        <v>0.46531680741301357</v>
+      </c>
+      <c r="BX15" s="24">
+        <v>-22.645011742484083</v>
       </c>
     </row>
   </sheetData>
@@ -2642,898 +2876,997 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BO15"/>
+  <dimension ref="A1:BV15"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="27" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="28"/>
       <c r="B2" s="28" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="G2" s="28" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="H2" s="28" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="J2" s="28" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="K2" s="28" t="s">
-        <v>133</v>
+        <v>145</v>
       </c>
       <c r="L2" s="28" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="M2" s="28" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="N2" s="28" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="O2" s="28" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="28" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="B3" s="28">
-        <v>0.054521965105579773</v>
+        <v>0.083981005461975733</v>
       </c>
       <c r="C3" s="28">
-        <v>0.0087381659051857241</v>
+        <v>-0.013025875553450028</v>
       </c>
       <c r="D3" s="28">
-        <v>0.034044670336057847</v>
+        <v>-0.042625821397913877</v>
       </c>
       <c r="E3" s="28">
-        <v>0.051499786078867404</v>
+        <v>-0.010234459917466299</v>
       </c>
       <c r="F3" s="28">
-        <v>-0.021297748608102407</v>
+        <v>-0.0056767840129877678</v>
       </c>
       <c r="G3" s="28">
-        <v>-0.0025092962742403468</v>
+        <v>0.0042333223263548159</v>
       </c>
       <c r="H3" s="28">
-        <v>0.038467656228066305</v>
+        <v>0.00085994414900109062</v>
       </c>
       <c r="I3" s="28">
-        <v>0.023405959119693232</v>
+        <v>0.031544217734642555</v>
       </c>
       <c r="J3" s="28">
-        <v>0.085767992949442873</v>
+        <v>0.054643743292424107</v>
       </c>
       <c r="K3" s="28">
-        <v>0.023918422158142161</v>
+        <v>0.10740039584203492</v>
       </c>
       <c r="L3" s="28">
-        <v>0.051496139974054278</v>
+        <v>-0.07010605191073116</v>
       </c>
       <c r="M3" s="28">
-        <v>0.05047732659856724</v>
+        <v>0.076927201919833932</v>
       </c>
       <c r="N3" s="28">
-        <v>-0.063491651352923451</v>
+        <v>-0.10413957751841024</v>
       </c>
       <c r="O3" s="28">
-        <v>-0.10134271699090541</v>
+        <v>-0.0075422890566660405</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="28" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="B4" s="28">
-        <v>0.82528911397957938</v>
+        <v>1.1087008515280277</v>
       </c>
       <c r="C4" s="28">
-        <v>0.14306905843177473</v>
+        <v>-0.17571733431587119</v>
       </c>
       <c r="D4" s="28">
-        <v>0.51694518216344165</v>
+        <v>-0.65178193316765387</v>
       </c>
       <c r="E4" s="28">
-        <v>0.76584536206629406</v>
+        <v>-0.15520428141502002</v>
       </c>
       <c r="F4" s="28">
-        <v>-0.34558270451770939</v>
+        <v>-0.08058027735869211</v>
       </c>
       <c r="G4" s="28">
-        <v>-0.039414889551806755</v>
+        <v>0.05704555050401084</v>
       </c>
       <c r="H4" s="28">
-        <v>0.60510081122426262</v>
+        <v>0.011585417483602433</v>
       </c>
       <c r="I4" s="28">
-        <v>0.37179463559749165</v>
+        <v>0.41653131091850132</v>
       </c>
       <c r="J4" s="28">
-        <v>1.2724756697820423</v>
+        <v>0.73356898138854332</v>
       </c>
       <c r="K4" s="28">
-        <v>0.38975658134373958</v>
+        <v>1.4118229198204679</v>
       </c>
       <c r="L4" s="28">
-        <v>0.82971966654131202</v>
+        <v>-1.2068948329331994</v>
       </c>
       <c r="M4" s="28">
-        <v>0.85457669571242667</v>
+        <v>1.1287112585535433</v>
       </c>
       <c r="N4" s="28">
-        <v>-1.165218151943928</v>
+        <v>-1.8648777267569554</v>
       </c>
       <c r="O4" s="28">
-        <v>-2.2175567145858297</v>
+        <v>-0.12680233041870331</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="31" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="32"/>
       <c r="B7" s="32" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
       <c r="D7" s="32" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="E7" s="32" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="F7" s="32" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="G7" s="32" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="H7" s="32" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="I7" s="32" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="J7" s="32" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="K7" s="32" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="L7" s="32" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="M7" s="32" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="N7" s="32" t="s">
-        <v>153</v>
+        <v>165</v>
+      </c>
+      <c r="O7" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="P7" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q7" s="32" t="s">
+        <v>168</v>
+      </c>
+      <c r="R7" s="32" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="32" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="B8" s="32">
-        <v>0.14321875147350022</v>
+        <v>0.14420487889875658</v>
       </c>
       <c r="C8" s="32">
-        <v>-0.1576186568195419</v>
+        <v>-0.38431446487096205</v>
       </c>
       <c r="D8" s="32">
-        <v>-0.070561987217539257</v>
+        <v>-0.13940429736519228</v>
       </c>
       <c r="E8" s="32">
-        <v>-0.045819241535478672</v>
+        <v>-0.071705317983206895</v>
       </c>
       <c r="F8" s="32">
-        <v>-0.067740174066673042</v>
+        <v>-0.048885953327709564</v>
       </c>
       <c r="G8" s="32">
-        <v>0.092035395355710481</v>
+        <v>0.015292208009507979</v>
       </c>
       <c r="H8" s="32">
-        <v>0.079459817016896389</v>
+        <v>-0.031603065930549457</v>
       </c>
       <c r="I8" s="32">
-        <v>-0.036462968056968026</v>
+        <v>-0.037776247502768756</v>
       </c>
       <c r="J8" s="32">
-        <v>0.047942570808665375</v>
+        <v>0.018215504632027923</v>
       </c>
       <c r="K8" s="32">
-        <v>-0.019054718395906611</v>
+        <v>0.11247558524376708</v>
       </c>
       <c r="L8" s="32">
-        <v>-0.02014727545009265</v>
+        <v>-0.0054854559570224337</v>
       </c>
       <c r="M8" s="32">
-        <v>0.064335154250444226</v>
+        <v>0.12429435012774817</v>
       </c>
       <c r="N8" s="32">
-        <v>0.065224472988095417</v>
+        <v>-0.019928639556743344</v>
+      </c>
+      <c r="O8" s="32">
+        <v>0.0091402186453130585</v>
+      </c>
+      <c r="P8" s="32">
+        <v>-0.089261419233351458</v>
+      </c>
+      <c r="Q8" s="32">
+        <v>-0.044398257559894183</v>
+      </c>
+      <c r="R8" s="32">
+        <v>-0.1496448495775497</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="32" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="B9" s="32">
-        <v>2.5511861038614758</v>
+        <v>2.3412927367952019</v>
       </c>
       <c r="C9" s="32">
-        <v>-3.7513107959363321</v>
+        <v>-13.702138237806297</v>
       </c>
       <c r="D9" s="32">
-        <v>-1.4032415504764733</v>
+        <v>-2.5695163563833279</v>
       </c>
       <c r="E9" s="32">
-        <v>-0.94645105674315699</v>
+        <v>-1.1553541436899621</v>
       </c>
       <c r="F9" s="32">
-        <v>-1.5381896339337993</v>
+        <v>-0.80718297338794798</v>
       </c>
       <c r="G9" s="32">
-        <v>1.6877232365985853</v>
+        <v>0.23232095090135799</v>
       </c>
       <c r="H9" s="32">
-        <v>1.5614732377634586</v>
+        <v>-0.51752811292429068</v>
       </c>
       <c r="I9" s="32">
-        <v>-0.86056653489403034</v>
+        <v>-0.64520822605081218</v>
       </c>
       <c r="J9" s="32">
-        <v>0.95662532080753138</v>
+        <v>0.28764868895543821</v>
       </c>
       <c r="K9" s="32">
-        <v>-0.41334961413173843</v>
+        <v>1.5897948439562328</v>
       </c>
       <c r="L9" s="32">
-        <v>-0.46561716572524148</v>
+        <v>-0.08750686682571493</v>
       </c>
       <c r="M9" s="32">
-        <v>1.3560251655486049</v>
+        <v>1.8122540019405389</v>
       </c>
       <c r="N9" s="32">
-        <v>1.9682297202418981</v>
+        <v>-0.35933445271756886</v>
+      </c>
+      <c r="O9" s="32">
+        <v>0.15244972572344567</v>
+      </c>
+      <c r="P9" s="32">
+        <v>-1.7994760832589158</v>
+      </c>
+      <c r="Q9" s="32">
+        <v>-0.82815742624283373</v>
+      </c>
+      <c r="R9" s="32">
+        <v>-3.3659591917873306</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="35" t="s">
-        <v>154</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="36"/>
       <c r="B13" s="36" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="E13" s="36" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
       <c r="F13" s="36" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="G13" s="36" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="H13" s="36" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
       <c r="I13" s="36" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
       <c r="J13" s="36" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="K13" s="36" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
       <c r="L13" s="36" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="M13" s="36" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="N13" s="36" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="O13" s="36" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="P13" s="36" t="s">
-        <v>171</v>
+        <v>187</v>
       </c>
       <c r="Q13" s="36" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="R13" s="36" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="S13" s="36" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
       <c r="T13" s="36" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
       <c r="U13" s="36" t="s">
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="V13" s="36" t="s">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="W13" s="36" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
       <c r="X13" s="36" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="Y13" s="36" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="Z13" s="36" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="AA13" s="36" t="s">
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="AB13" s="36" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="AC13" s="36" t="s">
-        <v>184</v>
+        <v>200</v>
       </c>
       <c r="AD13" s="36" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="AE13" s="36" t="s">
-        <v>186</v>
+        <v>202</v>
       </c>
       <c r="AF13" s="36" t="s">
-        <v>187</v>
+        <v>203</v>
       </c>
       <c r="AG13" s="36" t="s">
-        <v>188</v>
+        <v>204</v>
       </c>
       <c r="AH13" s="36" t="s">
-        <v>189</v>
+        <v>205</v>
       </c>
       <c r="AI13" s="36" t="s">
-        <v>190</v>
+        <v>206</v>
       </c>
       <c r="AJ13" s="36" t="s">
-        <v>191</v>
+        <v>207</v>
       </c>
       <c r="AK13" s="36" t="s">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="AL13" s="36" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
       <c r="AM13" s="36" t="s">
-        <v>194</v>
+        <v>210</v>
       </c>
       <c r="AN13" s="36" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="AO13" s="36" t="s">
-        <v>196</v>
+        <v>212</v>
       </c>
       <c r="AP13" s="36" t="s">
-        <v>197</v>
+        <v>213</v>
       </c>
       <c r="AQ13" s="36" t="s">
-        <v>198</v>
+        <v>214</v>
       </c>
       <c r="AR13" s="36" t="s">
-        <v>199</v>
+        <v>215</v>
       </c>
       <c r="AS13" s="36" t="s">
-        <v>200</v>
+        <v>216</v>
       </c>
       <c r="AT13" s="36" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="AU13" s="36" t="s">
-        <v>202</v>
+        <v>218</v>
       </c>
       <c r="AV13" s="36" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="AW13" s="36" t="s">
-        <v>204</v>
+        <v>220</v>
       </c>
       <c r="AX13" s="36" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
       <c r="AY13" s="36" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="AZ13" s="36" t="s">
-        <v>207</v>
+        <v>223</v>
       </c>
       <c r="BA13" s="36" t="s">
-        <v>208</v>
+        <v>224</v>
       </c>
       <c r="BB13" s="36" t="s">
-        <v>209</v>
+        <v>225</v>
       </c>
       <c r="BC13" s="36" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
       <c r="BD13" s="36" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="BE13" s="36" t="s">
-        <v>212</v>
+        <v>228</v>
       </c>
       <c r="BF13" s="36" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
       <c r="BG13" s="36" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="BH13" s="36" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
       <c r="BI13" s="36" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
       <c r="BJ13" s="36" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
       <c r="BK13" s="36" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
       <c r="BL13" s="36" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
       <c r="BM13" s="36" t="s">
-        <v>220</v>
+        <v>236</v>
       </c>
       <c r="BN13" s="36" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
       <c r="BO13" s="36" t="s">
-        <v>222</v>
+        <v>238</v>
+      </c>
+      <c r="BP13" s="36" t="s">
+        <v>239</v>
+      </c>
+      <c r="BQ13" s="36" t="s">
+        <v>240</v>
+      </c>
+      <c r="BR13" s="36" t="s">
+        <v>241</v>
+      </c>
+      <c r="BS13" s="36" t="s">
+        <v>242</v>
+      </c>
+      <c r="BT13" s="36" t="s">
+        <v>243</v>
+      </c>
+      <c r="BU13" s="36" t="s">
+        <v>244</v>
+      </c>
+      <c r="BV13" s="36" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="36" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="B14" s="36">
-        <v>-0.47610888495540721</v>
+        <v>-0.53355780381982532</v>
       </c>
       <c r="C14" s="36">
-        <v>-0.61814096678922148</v>
+        <v>-0.16834756089252628</v>
       </c>
       <c r="D14" s="36">
-        <v>-0.33490171559774196</v>
+        <v>-0.67436692349375349</v>
       </c>
       <c r="E14" s="36">
-        <v>-0.58922311363482649</v>
+        <v>-0.16607203933531123</v>
       </c>
       <c r="F14" s="36">
-        <v>-0.088588695101760984</v>
+        <v>-0.69655761960868312</v>
       </c>
       <c r="G14" s="36">
-        <v>-0.03111597340189487</v>
+        <v>-0.38578923630819079</v>
       </c>
       <c r="H14" s="36">
-        <v>-0.21570925079928399</v>
+        <v>-0.1192424556514044</v>
       </c>
       <c r="I14" s="36">
-        <v>-0.42002734802594915</v>
+        <v>0.24206442741283773</v>
       </c>
       <c r="J14" s="36">
-        <v>-0.049101753855349373</v>
+        <v>-0.6683637613022253</v>
       </c>
       <c r="K14" s="36">
-        <v>0.17222716555128634</v>
+        <v>-0.05821494662969251</v>
       </c>
       <c r="L14" s="36">
-        <v>-0.17825227335745081</v>
+        <v>-0.31719627977898174</v>
       </c>
       <c r="M14" s="36">
-        <v>-0.36961578845501053</v>
+        <v>-0.15791037426410104</v>
       </c>
       <c r="N14" s="36">
-        <v>-0.40081396527862984</v>
+        <v>0.00092570700680355555</v>
       </c>
       <c r="O14" s="36">
-        <v>-0.31294356029064668</v>
+        <v>0.018993600994860027</v>
       </c>
       <c r="P14" s="36">
-        <v>-0.38855817651078417</v>
+        <v>-0.18213744418676042</v>
       </c>
       <c r="Q14" s="36">
-        <v>-0.24565827543375757</v>
+        <v>-0.66187566241815332</v>
       </c>
       <c r="R14" s="36">
-        <v>-0.043661911847976242</v>
+        <v>-0.64714455058704601</v>
       </c>
       <c r="S14" s="36">
-        <v>0.088354238005792424</v>
+        <v>-0.29862263206660244</v>
       </c>
       <c r="T14" s="36">
-        <v>-0.19251342278006139</v>
+        <v>-0.10526764415869166</v>
       </c>
       <c r="U14" s="36">
-        <v>-0.087422757527402972</v>
+        <v>-0.15203663466031814</v>
       </c>
       <c r="V14" s="36">
-        <v>0.041881139296976733</v>
+        <v>-0.16703283426673987</v>
       </c>
       <c r="W14" s="36">
-        <v>0.016170890231761881</v>
+        <v>-0.15799224211752844</v>
       </c>
       <c r="X14" s="36">
-        <v>0.020066750613728035</v>
+        <v>-0.24442169261843505</v>
       </c>
       <c r="Y14" s="36">
-        <v>0.046366433009286223</v>
+        <v>-0.32849230520994432</v>
       </c>
       <c r="Z14" s="36">
-        <v>0.10381312060479619</v>
+        <v>-0.25309700194411039</v>
       </c>
       <c r="AA14" s="36">
-        <v>-0.11474425076188755</v>
+        <v>-0.34930322223315297</v>
       </c>
       <c r="AB14" s="36">
-        <v>-0.10936930433231223</v>
+        <v>-0.19854023323074232</v>
       </c>
       <c r="AC14" s="36">
-        <v>-0.040358625963431816</v>
+        <v>-0.18295834110285164</v>
       </c>
       <c r="AD14" s="36">
-        <v>0.063688358235488352</v>
+        <v>-0.025190292785205681</v>
       </c>
       <c r="AE14" s="36">
-        <v>0.17832464976882251</v>
+        <v>0.027577774426815638</v>
       </c>
       <c r="AF14" s="36">
-        <v>-0.065120498835254642</v>
+        <v>0.079721703194181426</v>
       </c>
       <c r="AG14" s="36">
-        <v>-0.015373286941922137</v>
+        <v>-0.002851689118528955</v>
       </c>
       <c r="AH14" s="36">
-        <v>0.033837943881216803</v>
+        <v>-0.080552223274316215</v>
       </c>
       <c r="AI14" s="36">
-        <v>0.011077452374908092</v>
+        <v>0.041282964265763333</v>
       </c>
       <c r="AJ14" s="36">
-        <v>-0.21143162792202896</v>
+        <v>0.022013348959327772</v>
       </c>
       <c r="AK14" s="36">
-        <v>-0.48544872199208994</v>
+        <v>-0.18026218456853749</v>
       </c>
       <c r="AL14" s="36">
-        <v>0.0074061206382730616</v>
+        <v>0.073905233812696119</v>
       </c>
       <c r="AM14" s="36">
-        <v>0.037865990972246077</v>
+        <v>-0.11483795585649265</v>
       </c>
       <c r="AN14" s="36">
-        <v>-0.025093255782213747</v>
+        <v>0.0060354098014325785</v>
       </c>
       <c r="AO14" s="36">
-        <v>0.027911617204847083</v>
+        <v>-0.075237922351775954</v>
       </c>
       <c r="AP14" s="36">
-        <v>-0.042046515190777678</v>
+        <v>-0.22845525042682141</v>
       </c>
       <c r="AQ14" s="36">
-        <v>-0.12969999338681476</v>
+        <v>-0.41830230496830867</v>
       </c>
       <c r="AR14" s="36">
-        <v>0.036203167000241065</v>
+        <v>-0.11315855672930986</v>
       </c>
       <c r="AS14" s="36">
-        <v>-0.37820695157136286</v>
+        <v>0.16892962811693374</v>
       </c>
       <c r="AT14" s="36">
-        <v>-0.3398242355704858</v>
+        <v>-0.021681979597550749</v>
       </c>
       <c r="AU14" s="36">
-        <v>-0.18818105125021295</v>
+        <v>0.034055937147087822</v>
       </c>
       <c r="AV14" s="36">
-        <v>-0.024379238464054487</v>
+        <v>-0.59850608254605264</v>
       </c>
       <c r="AW14" s="36">
-        <v>-0.011164301939764809</v>
+        <v>-0.40096880744443214</v>
       </c>
       <c r="AX14" s="36">
-        <v>-0.13362316852763534</v>
+        <v>-0.35146763488201838</v>
       </c>
       <c r="AY14" s="36">
-        <v>0.00218492555896177</v>
+        <v>-0.18123783739896726</v>
       </c>
       <c r="AZ14" s="36">
-        <v>-0.061916708098030515</v>
+        <v>-0.32180983493506621</v>
       </c>
       <c r="BA14" s="36">
-        <v>0.0082714105140270222</v>
+        <v>-0.11147366907706574</v>
       </c>
       <c r="BB14" s="36">
-        <v>-0.0052708214322179647</v>
+        <v>-0.23810715699115464</v>
       </c>
       <c r="BC14" s="36">
-        <v>-0.031659830904067821</v>
+        <v>-0.16652994669884624</v>
       </c>
       <c r="BD14" s="36">
-        <v>-0.10831028017081573</v>
+        <v>-0.11416376527799948</v>
       </c>
       <c r="BE14" s="36">
-        <v>-0.20870986989612839</v>
+        <v>0.15263394945800424</v>
       </c>
       <c r="BF14" s="36">
-        <v>-0.1122875725631223</v>
+        <v>-0.53910560364817561</v>
       </c>
       <c r="BG14" s="36">
-        <v>-0.35337816913413733</v>
+        <v>-0.65470092699038329</v>
       </c>
       <c r="BH14" s="36">
-        <v>-0.24556751313756497</v>
+        <v>-0.27006940546959834</v>
       </c>
       <c r="BI14" s="36">
-        <v>-0.36293286877743997</v>
+        <v>-0.55333650134203372</v>
       </c>
       <c r="BJ14" s="36">
-        <v>-0.30173451376106208</v>
+        <v>-0.28651530003653597</v>
       </c>
       <c r="BK14" s="36">
-        <v>-0.22664356824539256</v>
+        <v>-0.48831380749064529</v>
       </c>
       <c r="BL14" s="36">
-        <v>-0.19730902638418457</v>
+        <v>-0.2149794103923463</v>
       </c>
       <c r="BM14" s="36">
-        <v>-0.23425751483105889</v>
+        <v>-0.28867989043416442</v>
       </c>
       <c r="BN14" s="36">
-        <v>-0.079837979881094756</v>
+        <v>-0.34159305631281833</v>
       </c>
       <c r="BO14" s="36">
-        <v>0.082630219536645372</v>
+        <v>-0.17834520151717076</v>
+      </c>
+      <c r="BP14" s="36">
+        <v>-0.38524403439191279</v>
+      </c>
+      <c r="BQ14" s="36">
+        <v>-0.43474939818745784</v>
+      </c>
+      <c r="BR14" s="36">
+        <v>-0.52286290315598116</v>
+      </c>
+      <c r="BS14" s="36">
+        <v>-0.5764135136186932</v>
+      </c>
+      <c r="BT14" s="36">
+        <v>-0.44541191572395178</v>
+      </c>
+      <c r="BU14" s="36">
+        <v>-0.4229018581411767</v>
+      </c>
+      <c r="BV14" s="36">
+        <v>-0.27014987667091411</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="36" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="B15" s="36">
-        <v>-23.79333959773879</v>
+        <v>-28.218898560389853</v>
       </c>
       <c r="C15" s="36">
-        <v>-28.137630897929352</v>
+        <v>-4.8403461165008244</v>
       </c>
       <c r="D15" s="36">
-        <v>-11.897199348717246</v>
+        <v>-33.172579309118667</v>
       </c>
       <c r="E15" s="36">
-        <v>-26.438691438049823</v>
+        <v>-2.1605783722115204</v>
       </c>
       <c r="F15" s="36">
-        <v>-1.8525449476279541</v>
+        <v>-34.206519459101621</v>
       </c>
       <c r="G15" s="36">
-        <v>-0.60939809196093453</v>
+        <v>-7.902138079718255</v>
       </c>
       <c r="H15" s="36">
-        <v>-12.310208474529793</v>
+        <v>-1.910865903298874</v>
       </c>
       <c r="I15" s="36">
-        <v>-39.921979779895409</v>
+        <v>3.671035179814754</v>
       </c>
       <c r="J15" s="36">
-        <v>-0.88268990292313232</v>
+        <v>-42.71403293653271</v>
       </c>
       <c r="K15" s="36">
-        <v>2.4884718775849239</v>
+        <v>-1.112212629411323</v>
       </c>
       <c r="L15" s="36">
-        <v>-4.6669295740307435</v>
+        <v>-10.774727375654235</v>
       </c>
       <c r="M15" s="36">
-        <v>-26.560592334586342</v>
+        <v>-3.5009540501542129</v>
       </c>
       <c r="N15" s="36">
-        <v>-16.427621345226616</v>
+        <v>0.012815650199565026</v>
       </c>
       <c r="O15" s="36">
-        <v>-13.132086290380649</v>
+        <v>0.30452862789216606</v>
       </c>
       <c r="P15" s="36">
-        <v>-13.72226129077813</v>
+        <v>-6.0358846605676622</v>
       </c>
       <c r="Q15" s="36">
-        <v>-13.531886766087728</v>
+        <v>-59.888984810272966</v>
       </c>
       <c r="R15" s="36">
-        <v>-1.1939248794506758</v>
+        <v>-17.633036227677305</v>
       </c>
       <c r="S15" s="36">
-        <v>1.986029816691256</v>
+        <v>-6.2708906717990018</v>
       </c>
       <c r="T15" s="36">
-        <v>-4.5035593524378683</v>
+        <v>-1.854266923684591</v>
       </c>
       <c r="U15" s="36">
-        <v>-1.6959788838252798</v>
+        <v>-2.8638969319956966</v>
       </c>
       <c r="V15" s="36">
-        <v>0.79984956315934563</v>
+        <v>-2.7430087002976622</v>
       </c>
       <c r="W15" s="36">
-        <v>0.34093670799883075</v>
+        <v>-2.7034012231861531</v>
       </c>
       <c r="X15" s="36">
-        <v>0.36858680094212598</v>
+        <v>-7.0138547503832394</v>
       </c>
       <c r="Y15" s="36">
-        <v>0.82965610414057955</v>
+        <v>-7.0582247356138019</v>
       </c>
       <c r="Z15" s="36">
-        <v>1.7581790755527322</v>
+        <v>-6.1601566127525755</v>
       </c>
       <c r="AA15" s="36">
-        <v>-1.6894666604064608</v>
+        <v>-7.9345849728795033</v>
       </c>
       <c r="AB15" s="36">
-        <v>-2.2054386920098836</v>
+        <v>-3.1661468455397292</v>
       </c>
       <c r="AC15" s="36">
-        <v>-0.82915151289256306</v>
+        <v>-3.7759715952628521</v>
       </c>
       <c r="AD15" s="36">
-        <v>2.0623779991152813</v>
+        <v>-0.38276205710661554</v>
       </c>
       <c r="AE15" s="36">
-        <v>10.674597663821594</v>
+        <v>0.35157951015745476</v>
       </c>
       <c r="AF15" s="36">
-        <v>-1.8144720431404076</v>
+        <v>0.99926139603513564</v>
       </c>
       <c r="AG15" s="36">
-        <v>-0.32999204379225611</v>
+        <v>-0.044307932472694829</v>
       </c>
       <c r="AH15" s="36">
-        <v>0.86276410001634973</v>
+        <v>-1.2967149797588446</v>
       </c>
       <c r="AI15" s="36">
-        <v>0.3127851869237071</v>
+        <v>0.56463981816530295</v>
       </c>
       <c r="AJ15" s="36">
-        <v>-4.6061193228340604</v>
+        <v>0.28813129990104369</v>
       </c>
       <c r="AK15" s="36">
-        <v>-21.724232373623199</v>
+        <v>-3.2566908258495992</v>
       </c>
       <c r="AL15" s="36">
-        <v>0.22169301862262766</v>
+        <v>1.1276070232740163</v>
       </c>
       <c r="AM15" s="36">
-        <v>0.88102103067657433</v>
+        <v>-1.8937015178849763</v>
       </c>
       <c r="AN15" s="36">
-        <v>-0.86499491714155796</v>
+        <v>0.096449802932879525</v>
       </c>
       <c r="AO15" s="36">
-        <v>0.61410132265928186</v>
+        <v>-1.0800476949810747</v>
       </c>
       <c r="AP15" s="36">
-        <v>-0.9931578513326409</v>
+        <v>-16.488150769648385</v>
       </c>
       <c r="AQ15" s="36">
-        <v>-2.9924304320983546</v>
+        <v>-11.841864689717353</v>
       </c>
       <c r="AR15" s="36">
-        <v>0.90128933655328847</v>
+        <v>-2.5794315674655324</v>
       </c>
       <c r="AS15" s="36">
-        <v>-65.541803691497705</v>
+        <v>2.1824299325556513</v>
       </c>
       <c r="AT15" s="36">
-        <v>-10.03936998172636</v>
+        <v>-0.37510553263235341</v>
       </c>
       <c r="AU15" s="36">
-        <v>-5.2942052230864025</v>
+        <v>0.50704476311120961</v>
       </c>
       <c r="AV15" s="36">
-        <v>-0.5159471081868876</v>
+        <v>-66.821893939422722</v>
       </c>
       <c r="AW15" s="36">
-        <v>-0.26767392628205239</v>
+        <v>-6.6305714071571913</v>
       </c>
       <c r="AX15" s="36">
-        <v>-4.153054502686679</v>
+        <v>-8.8840031570436668</v>
       </c>
       <c r="AY15" s="36">
-        <v>0.054895366063453958</v>
+        <v>-4.0105212027401969</v>
       </c>
       <c r="AZ15" s="36">
-        <v>-1.5390839088754156</v>
+        <v>-16.46959879026014</v>
       </c>
       <c r="BA15" s="36">
-        <v>0.21054595562375542</v>
+        <v>-2.4557616150836155</v>
       </c>
       <c r="BB15" s="36">
-        <v>-0.11246158682190688</v>
+        <v>-5.7016564811723951</v>
       </c>
       <c r="BC15" s="36">
-        <v>-0.71887451637741828</v>
+        <v>-4.1430259304588368</v>
       </c>
       <c r="BD15" s="36">
-        <v>-3.2480476704737322</v>
+        <v>-2.5226854213810928</v>
       </c>
       <c r="BE15" s="36">
-        <v>-5.8806540093625488</v>
+        <v>1.9601370170563579</v>
       </c>
       <c r="BF15" s="36">
-        <v>-10.355598643352838</v>
+        <v>-22.579658752159133</v>
       </c>
       <c r="BG15" s="36">
-        <v>-13.97968404265311</v>
+        <v>-28.957058837656891</v>
       </c>
       <c r="BH15" s="36">
-        <v>-8.2628230720652649</v>
+        <v>-4.8997651177223904</v>
       </c>
       <c r="BI15" s="36">
-        <v>-16.519039221653173</v>
+        <v>-66.991436560130552</v>
       </c>
       <c r="BJ15" s="36">
-        <v>-18.457585121340429</v>
+        <v>-7.1942298459702112</v>
       </c>
       <c r="BK15" s="36">
-        <v>-8.4392757986213169</v>
+        <v>-28.816345142223252</v>
       </c>
       <c r="BL15" s="36">
-        <v>-6.8400612828341965</v>
+        <v>-4.4554125553889055</v>
       </c>
       <c r="BM15" s="36">
-        <v>-10.340111754390746</v>
+        <v>-8.5383725554638694</v>
       </c>
       <c r="BN15" s="36">
-        <v>-3.3990432155134376</v>
+        <v>-9.6593599637753371</v>
       </c>
       <c r="BO15" s="36">
-        <v>3.8187722643086581</v>
+        <v>-3.9415864438179584</v>
+      </c>
+      <c r="BP15" s="36">
+        <v>-11.297509454134099</v>
+      </c>
+      <c r="BQ15" s="36">
+        <v>-16.052096040690394</v>
+      </c>
+      <c r="BR15" s="36">
+        <v>-17.924787548247373</v>
+      </c>
+      <c r="BS15" s="36">
+        <v>-21.152535545418672</v>
+      </c>
+      <c r="BT15" s="36">
+        <v>-14.86103588150311</v>
+      </c>
+      <c r="BU15" s="36">
+        <v>-14.958961491743304</v>
+      </c>
+      <c r="BV15" s="36">
+        <v>-8.501529122123145</v>
       </c>
     </row>
   </sheetData>
@@ -3542,583 +3875,754 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AU15"/>
+  <dimension ref="A1:BJ15"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="39" t="s">
-        <v>223</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="40"/>
       <c r="B2" s="40" t="s">
-        <v>226</v>
+        <v>249</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>227</v>
+        <v>250</v>
       </c>
       <c r="D2" s="40" t="s">
-        <v>228</v>
+        <v>251</v>
       </c>
       <c r="E2" s="40" t="s">
-        <v>229</v>
+        <v>252</v>
       </c>
       <c r="F2" s="40" t="s">
-        <v>230</v>
+        <v>253</v>
       </c>
       <c r="G2" s="40" t="s">
-        <v>231</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="40" t="s">
-        <v>224</v>
+        <v>247</v>
       </c>
       <c r="B3" s="40">
-        <v>0.054521965105579773</v>
+        <v>0.053143017531737224</v>
       </c>
       <c r="C3" s="40">
-        <v>-0.088546776187542087</v>
+        <v>-0.010234459917466299</v>
       </c>
       <c r="D3" s="40">
-        <v>-0.075822186209696441</v>
+        <v>-0.063793780081387419</v>
       </c>
       <c r="E3" s="40">
-        <v>0.05047732659856724</v>
+        <v>0.012836778343008559</v>
       </c>
       <c r="F3" s="40">
-        <v>0.04317559990045261</v>
+        <v>0.076927201919833932</v>
       </c>
       <c r="G3" s="40">
-        <v>0.076406335660846925</v>
+        <v>-0.0075422890566660405</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="40" t="s">
-        <v>225</v>
+        <v>248</v>
       </c>
       <c r="B4" s="40">
-        <v>0.82528911397957938</v>
+        <v>0.70436068102750038</v>
       </c>
       <c r="C4" s="40">
-        <v>-1.5766655770578781</v>
+        <v>-0.15520428141502002</v>
       </c>
       <c r="D4" s="40">
-        <v>-1.3895587226050552</v>
+        <v>-0.94204820668665001</v>
       </c>
       <c r="E4" s="40">
-        <v>0.85457669571242667</v>
+        <v>0.18475769038183848</v>
       </c>
       <c r="F4" s="40">
-        <v>0.74194285038838914</v>
+        <v>1.1287112585535433</v>
       </c>
       <c r="G4" s="40">
-        <v>1.3540300232200393</v>
+        <v>-0.12680233041870331</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="43" t="s">
-        <v>232</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="44"/>
       <c r="B7" s="44" t="s">
-        <v>235</v>
+        <v>258</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>236</v>
+        <v>259</v>
       </c>
       <c r="D7" s="44" t="s">
-        <v>237</v>
+        <v>260</v>
       </c>
       <c r="E7" s="44" t="s">
-        <v>238</v>
+        <v>261</v>
       </c>
       <c r="F7" s="44" t="s">
-        <v>239</v>
+        <v>262</v>
       </c>
       <c r="G7" s="44" t="s">
-        <v>240</v>
+        <v>263</v>
+      </c>
+      <c r="H7" s="44" t="s">
+        <v>264</v>
+      </c>
+      <c r="I7" s="44" t="s">
+        <v>265</v>
+      </c>
+      <c r="J7" s="44" t="s">
+        <v>266</v>
+      </c>
+      <c r="K7" s="44" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="44" t="s">
-        <v>233</v>
+        <v>256</v>
       </c>
       <c r="B8" s="44">
-        <v>0.14321875147350022</v>
+        <v>0.14420487889875658</v>
       </c>
       <c r="C8" s="44">
-        <v>-0.070561987217539257</v>
+        <v>0.17019563014822001</v>
       </c>
       <c r="D8" s="44">
-        <v>-0.067740174066673042</v>
+        <v>-0.071705317983206895</v>
       </c>
       <c r="E8" s="44">
-        <v>0.079459817016896389</v>
+        <v>0.015292208009507979</v>
       </c>
       <c r="F8" s="44">
-        <v>-0.036570303899151613</v>
+        <v>-0.088203520784450651</v>
       </c>
       <c r="G8" s="44">
-        <v>0.03552703880599492</v>
+        <v>-0.04335128997796811</v>
+      </c>
+      <c r="H8" s="44">
+        <v>0.0091402186453130585</v>
+      </c>
+      <c r="I8" s="44">
+        <v>-0.044398257559894183</v>
+      </c>
+      <c r="J8" s="44">
+        <v>0.026094157395636752</v>
+      </c>
+      <c r="K8" s="44">
+        <v>-0.70277563076210114</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="44" t="s">
-        <v>234</v>
+        <v>257</v>
       </c>
       <c r="B9" s="44">
-        <v>2.5511861038614758</v>
+        <v>2.3412927367952019</v>
       </c>
       <c r="C9" s="44">
-        <v>-1.4032415504764733</v>
+        <v>2.3949246130938042</v>
       </c>
       <c r="D9" s="44">
-        <v>-1.5381896339337993</v>
+        <v>-1.1553541436899621</v>
       </c>
       <c r="E9" s="44">
-        <v>1.5614732377634586</v>
+        <v>0.23232095090135799</v>
       </c>
       <c r="F9" s="44">
-        <v>-0.8476345020862105</v>
+        <v>-1.6238685534855744</v>
       </c>
       <c r="G9" s="44">
-        <v>0.8084689076461643</v>
+        <v>-0.75817046356599682</v>
+      </c>
+      <c r="H9" s="44">
+        <v>0.15244972572344567</v>
+      </c>
+      <c r="I9" s="44">
+        <v>-0.82815742624283373</v>
+      </c>
+      <c r="J9" s="44">
+        <v>0.47126308037296438</v>
+      </c>
+      <c r="K9" s="44">
+        <v>-26.413103445171018</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="47" t="s">
-        <v>241</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="48"/>
       <c r="B13" s="48" t="s">
-        <v>244</v>
+        <v>271</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>245</v>
+        <v>272</v>
       </c>
       <c r="D13" s="48" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="E13" s="48" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
       <c r="F13" s="48" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="G13" s="48" t="s">
-        <v>249</v>
+        <v>276</v>
       </c>
       <c r="H13" s="48" t="s">
-        <v>250</v>
+        <v>277</v>
       </c>
       <c r="I13" s="48" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
       <c r="J13" s="48" t="s">
-        <v>252</v>
+        <v>279</v>
       </c>
       <c r="K13" s="48" t="s">
-        <v>253</v>
+        <v>280</v>
       </c>
       <c r="L13" s="48" t="s">
-        <v>254</v>
+        <v>281</v>
       </c>
       <c r="M13" s="48" t="s">
-        <v>255</v>
+        <v>282</v>
       </c>
       <c r="N13" s="48" t="s">
-        <v>256</v>
+        <v>283</v>
       </c>
       <c r="O13" s="48" t="s">
-        <v>257</v>
+        <v>284</v>
       </c>
       <c r="P13" s="48" t="s">
-        <v>258</v>
+        <v>285</v>
       </c>
       <c r="Q13" s="48" t="s">
-        <v>259</v>
+        <v>286</v>
       </c>
       <c r="R13" s="48" t="s">
-        <v>260</v>
+        <v>287</v>
       </c>
       <c r="S13" s="48" t="s">
-        <v>261</v>
+        <v>288</v>
       </c>
       <c r="T13" s="48" t="s">
-        <v>262</v>
+        <v>289</v>
       </c>
       <c r="U13" s="48" t="s">
-        <v>263</v>
+        <v>290</v>
       </c>
       <c r="V13" s="48" t="s">
-        <v>264</v>
+        <v>291</v>
       </c>
       <c r="W13" s="48" t="s">
-        <v>265</v>
+        <v>292</v>
       </c>
       <c r="X13" s="48" t="s">
-        <v>266</v>
+        <v>293</v>
       </c>
       <c r="Y13" s="48" t="s">
-        <v>267</v>
+        <v>294</v>
       </c>
       <c r="Z13" s="48" t="s">
-        <v>268</v>
+        <v>295</v>
       </c>
       <c r="AA13" s="48" t="s">
-        <v>269</v>
+        <v>296</v>
       </c>
       <c r="AB13" s="48" t="s">
-        <v>270</v>
+        <v>297</v>
       </c>
       <c r="AC13" s="48" t="s">
-        <v>271</v>
+        <v>298</v>
       </c>
       <c r="AD13" s="48" t="s">
-        <v>272</v>
+        <v>299</v>
       </c>
       <c r="AE13" s="48" t="s">
-        <v>273</v>
+        <v>300</v>
       </c>
       <c r="AF13" s="48" t="s">
-        <v>274</v>
+        <v>301</v>
       </c>
       <c r="AG13" s="48" t="s">
-        <v>275</v>
+        <v>302</v>
       </c>
       <c r="AH13" s="48" t="s">
-        <v>276</v>
+        <v>303</v>
       </c>
       <c r="AI13" s="48" t="s">
-        <v>277</v>
+        <v>304</v>
       </c>
       <c r="AJ13" s="48" t="s">
-        <v>278</v>
+        <v>305</v>
       </c>
       <c r="AK13" s="48" t="s">
-        <v>279</v>
+        <v>306</v>
       </c>
       <c r="AL13" s="48" t="s">
-        <v>280</v>
+        <v>307</v>
       </c>
       <c r="AM13" s="48" t="s">
-        <v>281</v>
+        <v>308</v>
       </c>
       <c r="AN13" s="48" t="s">
-        <v>282</v>
+        <v>309</v>
       </c>
       <c r="AO13" s="48" t="s">
-        <v>283</v>
+        <v>310</v>
       </c>
       <c r="AP13" s="48" t="s">
-        <v>284</v>
+        <v>311</v>
       </c>
       <c r="AQ13" s="48" t="s">
-        <v>285</v>
+        <v>312</v>
       </c>
       <c r="AR13" s="48" t="s">
-        <v>286</v>
+        <v>313</v>
       </c>
       <c r="AS13" s="48" t="s">
-        <v>287</v>
+        <v>314</v>
       </c>
       <c r="AT13" s="48" t="s">
-        <v>288</v>
+        <v>315</v>
       </c>
       <c r="AU13" s="48" t="s">
-        <v>289</v>
+        <v>316</v>
+      </c>
+      <c r="AV13" s="48" t="s">
+        <v>317</v>
+      </c>
+      <c r="AW13" s="48" t="s">
+        <v>318</v>
+      </c>
+      <c r="AX13" s="48" t="s">
+        <v>319</v>
+      </c>
+      <c r="AY13" s="48" t="s">
+        <v>320</v>
+      </c>
+      <c r="AZ13" s="48" t="s">
+        <v>321</v>
+      </c>
+      <c r="BA13" s="48" t="s">
+        <v>322</v>
+      </c>
+      <c r="BB13" s="48" t="s">
+        <v>323</v>
+      </c>
+      <c r="BC13" s="48" t="s">
+        <v>324</v>
+      </c>
+      <c r="BD13" s="48" t="s">
+        <v>325</v>
+      </c>
+      <c r="BE13" s="48" t="s">
+        <v>326</v>
+      </c>
+      <c r="BF13" s="48" t="s">
+        <v>327</v>
+      </c>
+      <c r="BG13" s="48" t="s">
+        <v>328</v>
+      </c>
+      <c r="BH13" s="48" t="s">
+        <v>329</v>
+      </c>
+      <c r="BI13" s="48" t="s">
+        <v>330</v>
+      </c>
+      <c r="BJ13" s="48" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="48" t="s">
-        <v>242</v>
+        <v>269</v>
       </c>
       <c r="B14" s="48">
-        <v>0.66962679906595168</v>
+        <v>0.49518170056294702</v>
       </c>
       <c r="C14" s="48">
-        <v>0.13362446219824239</v>
+        <v>0.43660330496016997</v>
       </c>
       <c r="D14" s="48">
-        <v>-2.2166799685721577</v>
+        <v>0.40247902674893671</v>
       </c>
       <c r="E14" s="48">
-        <v>0.0033577666985339372</v>
+        <v>0.33778266276375463</v>
       </c>
       <c r="F14" s="48">
-        <v>0.46095915825999284</v>
+        <v>0.66655483734855214</v>
       </c>
       <c r="G14" s="48">
-        <v>-0.03111597340189487</v>
+        <v>0.40244288183093951</v>
       </c>
       <c r="H14" s="48">
-        <v>-0.012899140648568369</v>
+        <v>0.061000701347620312</v>
       </c>
       <c r="I14" s="48">
-        <v>-0.088655848548528871</v>
+        <v>0.24206442741283773</v>
       </c>
       <c r="J14" s="48">
-        <v>0.029350881801036122</v>
+        <v>-0.05821494662969251</v>
       </c>
       <c r="K14" s="48">
-        <v>0.36696500674523652</v>
+        <v>0.14897427922432865</v>
       </c>
       <c r="L14" s="48">
-        <v>-0.014189755919901792</v>
+        <v>0.00092570700680355555</v>
       </c>
       <c r="M14" s="48">
-        <v>-0.095461834978672278</v>
+        <v>1.5874525706655915</v>
       </c>
       <c r="N14" s="48">
-        <v>0.072397055807492949</v>
+        <v>0.29921784466845747</v>
       </c>
       <c r="O14" s="48">
-        <v>-0.043661911847976242</v>
+        <v>0.055490230771631399</v>
       </c>
       <c r="P14" s="48">
-        <v>0.24584638669417613</v>
+        <v>-0.12390894052888557</v>
       </c>
       <c r="Q14" s="48">
-        <v>0.30442226496706593</v>
+        <v>-0.13578999200336792</v>
       </c>
       <c r="R14" s="48">
-        <v>-0.05885195336910104</v>
+        <v>0.018916687568856227</v>
       </c>
       <c r="S14" s="48">
-        <v>-0.026840911976420356</v>
+        <v>-0.024419501588821835</v>
       </c>
       <c r="T14" s="48">
-        <v>-0.040358625963431816</v>
+        <v>0.063386533603545903</v>
       </c>
       <c r="U14" s="48">
-        <v>0.17832464976882251</v>
+        <v>0.41105129988779354</v>
       </c>
       <c r="V14" s="48">
-        <v>-0.015373286941922137</v>
+        <v>0.11962688664925708</v>
       </c>
       <c r="W14" s="48">
-        <v>0.011077452374908092</v>
+        <v>0.23307218060099349</v>
       </c>
       <c r="X14" s="48">
-        <v>0.36171660393626837</v>
+        <v>0.10889007735635536</v>
       </c>
       <c r="Y14" s="48">
-        <v>0.0074061206382730616</v>
+        <v>0.25827484068170958</v>
       </c>
       <c r="Z14" s="48">
-        <v>-0.025093255782213747</v>
+        <v>0.26815435748222377</v>
       </c>
       <c r="AA14" s="48">
-        <v>-0.042046515190777678</v>
+        <v>-0.09722021056468616</v>
       </c>
       <c r="AB14" s="48">
-        <v>0.036203167000241065</v>
+        <v>-0.002851689118528955</v>
       </c>
       <c r="AC14" s="48">
-        <v>0.62959165601735156</v>
+        <v>-0.066343009490128058</v>
       </c>
       <c r="AD14" s="48">
-        <v>0.091506883198144817</v>
+        <v>-0.088175920006145547</v>
       </c>
       <c r="AE14" s="48">
-        <v>-0.024379238464054487</v>
+        <v>-0.075237922351775954</v>
       </c>
       <c r="AF14" s="48">
-        <v>0.51022042714299998</v>
+        <v>0.18368003790265566</v>
       </c>
       <c r="AG14" s="48">
-        <v>0.00218492555896177</v>
+        <v>0.08205232765447884</v>
       </c>
       <c r="AH14" s="48">
-        <v>0.0082714105140270222</v>
+        <v>0.16892962811693374</v>
       </c>
       <c r="AI14" s="48">
-        <v>-0.031659830904067821</v>
+        <v>0.034055937147087822</v>
       </c>
       <c r="AJ14" s="48">
-        <v>-0.011542843689957172</v>
+        <v>-0.022726000888747822</v>
       </c>
       <c r="AK14" s="48">
-        <v>0.64993866141563739</v>
+        <v>-0.038920704285130947</v>
       </c>
       <c r="AL14" s="48">
-        <v>0.14339970021016785</v>
+        <v>0.10255500476472745</v>
       </c>
       <c r="AM14" s="48">
-        <v>-0.059624582928452186</v>
+        <v>0.092348078919478299</v>
       </c>
       <c r="AN14" s="48">
-        <v>0.043933604013526528</v>
+        <v>0.26929472764911699</v>
       </c>
       <c r="AO14" s="48">
-        <v>3.9904766919570602</v>
+        <v>0.13585726223229622</v>
       </c>
       <c r="AP14" s="48">
-        <v>-0.018699527545565892</v>
+        <v>0.093743874056586129</v>
       </c>
       <c r="AQ14" s="48">
-        <v>0.034408885251043825</v>
+        <v>4.2536005140793574</v>
       </c>
       <c r="AR14" s="48">
-        <v>0.53146107928339625</v>
+        <v>0.15263394945800424</v>
       </c>
       <c r="AS14" s="48">
-        <v>0.1228193286704034</v>
+        <v>0.15853831327706275</v>
       </c>
       <c r="AT14" s="48">
-        <v>0.082630219536645372</v>
+        <v>0.0030973285978477261</v>
       </c>
       <c r="AU14" s="48">
-        <v>-0.51453561825376026</v>
+        <v>0.061620758555066296</v>
+      </c>
+      <c r="AV14" s="48">
+        <v>0.12832135477778733</v>
+      </c>
+      <c r="AW14" s="48">
+        <v>0.11946085097370376</v>
+      </c>
+      <c r="AX14" s="48">
+        <v>0.72129957436028647</v>
+      </c>
+      <c r="AY14" s="48">
+        <v>1.2370438771579466</v>
+      </c>
+      <c r="AZ14" s="48">
+        <v>0.046314345029220605</v>
+      </c>
+      <c r="BA14" s="48">
+        <v>0.094534890745803429</v>
+      </c>
+      <c r="BB14" s="48">
+        <v>0.09869576370038069</v>
+      </c>
+      <c r="BC14" s="48">
+        <v>-0.090913474955031659</v>
+      </c>
+      <c r="BD14" s="48">
+        <v>0.073170095455457662</v>
+      </c>
+      <c r="BE14" s="48">
+        <v>0.15833744247497936</v>
+      </c>
+      <c r="BF14" s="48">
+        <v>3.2130627080259062</v>
+      </c>
+      <c r="BG14" s="48">
+        <v>0.47831703403700088</v>
+      </c>
+      <c r="BH14" s="48">
+        <v>0.11958738203699448</v>
+      </c>
+      <c r="BI14" s="48">
+        <v>0.016090794687141585</v>
+      </c>
+      <c r="BJ14" s="48">
+        <v>-0.61371963667920859</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="48" t="s">
-        <v>243</v>
+        <v>270</v>
       </c>
       <c r="B15" s="48">
-        <v>6.2903470233308614</v>
+        <v>5.2757919361774306</v>
       </c>
       <c r="C15" s="48">
-        <v>2.3653407081514324</v>
+        <v>5.12270890202758</v>
       </c>
       <c r="D15" s="48">
-        <v>-1.6045052331929064</v>
+        <v>5.5110546755875731</v>
       </c>
       <c r="E15" s="48">
-        <v>0.044467710136045405</v>
+        <v>2.7578442892503099</v>
       </c>
       <c r="F15" s="48">
-        <v>5.4430853880501422</v>
+        <v>3.8333227619670605</v>
       </c>
       <c r="G15" s="48">
-        <v>-0.60939809196093453</v>
+        <v>7.7384165682239097</v>
       </c>
       <c r="H15" s="48">
-        <v>-0.7440442222618262</v>
+        <v>0.64951831536089366</v>
       </c>
       <c r="I15" s="48">
-        <v>-1.6488016416527158</v>
+        <v>3.671035179814754</v>
       </c>
       <c r="J15" s="48">
-        <v>0.76903094036502806</v>
+        <v>-1.112212629411323</v>
       </c>
       <c r="K15" s="48">
-        <v>6.1189460068577137</v>
+        <v>2.0008293447432481</v>
       </c>
       <c r="L15" s="48">
-        <v>-0.77745409527881604</v>
+        <v>0.012815650199565026</v>
       </c>
       <c r="M15" s="48">
-        <v>-2.546825420085689</v>
+        <v>20.804839807581164</v>
       </c>
       <c r="N15" s="48">
-        <v>2.1685100591948494</v>
+        <v>3.3720019659199938</v>
       </c>
       <c r="O15" s="48">
-        <v>-1.1939248794506758</v>
+        <v>0.87254745075401619</v>
       </c>
       <c r="P15" s="48">
-        <v>3.0585956890836301</v>
+        <v>-1.9455360921607725</v>
       </c>
       <c r="Q15" s="48">
-        <v>15.522374012007159</v>
+        <v>-0.32191194092089898</v>
       </c>
       <c r="R15" s="48">
-        <v>-1.4168367130232336</v>
+        <v>0.25586551324184376</v>
       </c>
       <c r="S15" s="48">
-        <v>-0.50643387938617401</v>
+        <v>-0.4805192613622315</v>
       </c>
       <c r="T15" s="48">
-        <v>-0.82915151289256306</v>
+        <v>0.81491090864584914</v>
       </c>
       <c r="U15" s="48">
-        <v>10.674597663821594</v>
+        <v>3.8174753986433485</v>
       </c>
       <c r="V15" s="48">
-        <v>-0.32999204379225611</v>
+        <v>3.6108759868243294</v>
       </c>
       <c r="W15" s="48">
-        <v>0.3127851869237071</v>
+        <v>2.3714615937811674</v>
       </c>
       <c r="X15" s="48">
-        <v>9.2500018648698745</v>
+        <v>1.5535018350320537</v>
       </c>
       <c r="Y15" s="48">
-        <v>0.22169301862262766</v>
+        <v>3.7878097717008394</v>
       </c>
       <c r="Z15" s="48">
-        <v>-0.86499491714155796</v>
+        <v>1.9327126693475385</v>
       </c>
       <c r="AA15" s="48">
-        <v>-0.9931578513326409</v>
+        <v>-1.4973924154826939</v>
       </c>
       <c r="AB15" s="48">
-        <v>0.90128933655328847</v>
+        <v>-0.044307932472694829</v>
       </c>
       <c r="AC15" s="48">
-        <v>11.371774700335159</v>
+        <v>-1.0402522161315013</v>
       </c>
       <c r="AD15" s="48">
-        <v>1.4496908423054604</v>
+        <v>-1.6325345221454532</v>
       </c>
       <c r="AE15" s="48">
-        <v>-0.5159471081868876</v>
+        <v>-1.0800476949810747</v>
       </c>
       <c r="AF15" s="48">
-        <v>7.4354299324933688</v>
+        <v>9.0227034262663501</v>
       </c>
       <c r="AG15" s="48">
-        <v>0.054895366063453958</v>
+        <v>4.2406728307232635</v>
       </c>
       <c r="AH15" s="48">
-        <v>0.21054595562375542</v>
+        <v>2.1824299325556513</v>
       </c>
       <c r="AI15" s="48">
-        <v>-0.71887451637741828</v>
+        <v>0.50704476311120961</v>
       </c>
       <c r="AJ15" s="48">
-        <v>-0.33938541480762274</v>
+        <v>-0.11052721339930192</v>
       </c>
       <c r="AK15" s="48">
-        <v>26.739782456850698</v>
+        <v>-0.73400822391863618</v>
       </c>
       <c r="AL15" s="48">
-        <v>7.0314444000588567</v>
+        <v>1.2928952079222877</v>
       </c>
       <c r="AM15" s="48">
-        <v>-1.5715631747374008</v>
+        <v>1.4831038104250389</v>
       </c>
       <c r="AN15" s="48">
-        <v>1.0539250714192765</v>
+        <v>4.2052775292397113</v>
       </c>
       <c r="AO15" s="48">
-        <v>2.8635183335557635</v>
+        <v>2.1928990722184047</v>
       </c>
       <c r="AP15" s="48">
-        <v>-1.0751371546216089</v>
+        <v>1.5936698748363416</v>
       </c>
       <c r="AQ15" s="48">
-        <v>0.85026228636205692</v>
+        <v>3.2287534897771093</v>
       </c>
       <c r="AR15" s="48">
-        <v>6.2881710940480522</v>
+        <v>1.9601370170563579</v>
       </c>
       <c r="AS15" s="48">
-        <v>3.4731630142663676</v>
+        <v>2.4379253802873579</v>
       </c>
       <c r="AT15" s="48">
-        <v>3.8187722643086581</v>
+        <v>0.041687198411506872</v>
       </c>
       <c r="AU15" s="48">
-        <v>-22.892776701289684</v>
+        <v>1.5903176832129493</v>
+      </c>
+      <c r="AV15" s="48">
+        <v>3.0678684791282471</v>
+      </c>
+      <c r="AW15" s="48">
+        <v>1.9828580554372954</v>
+      </c>
+      <c r="AX15" s="48">
+        <v>7.6732092679835713</v>
+      </c>
+      <c r="AY15" s="48">
+        <v>16.463995213534297</v>
+      </c>
+      <c r="AZ15" s="48">
+        <v>0.89229055571995908</v>
+      </c>
+      <c r="BA15" s="48">
+        <v>1.4918734785894916</v>
+      </c>
+      <c r="BB15" s="48">
+        <v>1.5730436655018905</v>
+      </c>
+      <c r="BC15" s="48">
+        <v>-1.8111827858865415</v>
+      </c>
+      <c r="BD15" s="48">
+        <v>1.7053284187021134</v>
+      </c>
+      <c r="BE15" s="48">
+        <v>2.5575079326147434</v>
+      </c>
+      <c r="BF15" s="48">
+        <v>2.016310711734187</v>
+      </c>
+      <c r="BG15" s="48">
+        <v>5.8815882521741951</v>
+      </c>
+      <c r="BH15" s="48">
+        <v>2.1960558592255399</v>
+      </c>
+      <c r="BI15" s="48">
+        <v>0.46531680741301357</v>
+      </c>
+      <c r="BJ15" s="48">
+        <v>-22.645011742484083</v>
       </c>
     </row>
   </sheetData>

</xml_diff>